<commit_message>
updated ets to calibrate elec
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\New Mexico\NM-eps\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738849F8-3EF3-4804-8F67-3336470FA6D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ECEA4D-840D-4A7B-915E-AE30DEFF964C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="450" yWindow="540" windowWidth="19750" windowHeight="13570" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,14 +214,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,11 +249,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -579,18 +570,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -598,77 +589,77 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -689,17 +680,17 @@
   </sheetPr>
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1">
@@ -796,7 +787,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -894,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -992,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1188,105 +1179,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AF6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1384,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1482,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1580,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1678,7 +1669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1874,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1972,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2070,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2168,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>

</xml_diff>